<commit_message>
Modification wireframe et mise a jour du journal
</commit_message>
<xml_diff>
--- a/Documents/Journal.xlsx
+++ b/Documents/Journal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Anel</t>
   </si>
@@ -33,7 +33,25 @@
     <t>Absent</t>
   </si>
   <si>
-    <t>Finition maquette, création des templates sur photoshop, création logo</t>
+    <t>Creation maquette, création des templates sur photoshop, création logo</t>
+  </si>
+  <si>
+    <t>Finition maquette et repartition du travail</t>
+  </si>
+  <si>
+    <t>Recherche de QCM et de templates</t>
+  </si>
+  <si>
+    <t>Analyse des sites et compléter la grille d'évaluation</t>
+  </si>
+  <si>
+    <t>Conception du Moodboard, wireframe balsamiq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synthèse de l'analyse, analyse des 2 derniers templates du sites de façon moins détaillée </t>
+  </si>
+  <si>
+    <t>Création d'un template complet</t>
   </si>
 </sst>
 </file>
@@ -69,10 +87,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -354,21 +375,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="107.85546875" customWidth="1"/>
     <col min="3" max="3" width="123" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
@@ -379,14 +400,63 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43107</v>
+      <c r="A2" s="2">
+        <v>43444</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>43446</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>43451</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>43107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>43109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>43114</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>